<commit_message>
Ajoute les donnees dans le programme arduino
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="220">
   <si>
     <t xml:space="preserve">8f6735e5</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t xml:space="preserve">des exemples dans les donnees, a completer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000000</t>
   </si>
 </sst>
 </file>
@@ -845,16 +848,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -890,14 +889,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -910,7 +901,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5736,139 +5735,116 @@
       <c r="A901" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B901" s="2"/>
     </row>
     <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A902" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B902" s="2"/>
     </row>
     <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A903" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B903" s="2"/>
     </row>
     <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A904" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B904" s="2"/>
     </row>
     <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A905" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B905" s="2"/>
     </row>
     <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A906" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B906" s="2"/>
     </row>
     <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A907" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B907" s="2"/>
     </row>
     <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A908" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B908" s="2"/>
     </row>
     <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A909" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B909" s="2"/>
     </row>
     <row r="910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A910" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B910" s="2"/>
     </row>
     <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A911" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B911" s="2"/>
     </row>
     <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A912" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B912" s="2"/>
     </row>
     <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A913" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B913" s="2"/>
     </row>
     <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A914" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B914" s="2"/>
     </row>
     <row r="915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A915" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B915" s="2"/>
     </row>
     <row r="916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A916" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B916" s="2"/>
     </row>
     <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B917" s="2"/>
     </row>
     <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A918" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B918" s="2"/>
     </row>
     <row r="919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A919" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B919" s="2"/>
     </row>
     <row r="920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A920" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B920" s="2"/>
     </row>
     <row r="921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B921" s="2"/>
     </row>
     <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A922" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B922" s="2"/>
     </row>
     <row r="923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A923" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B923" s="2"/>
     </row>
     <row r="924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A924" s="0" t="s">
@@ -6270,163 +6246,136 @@
       <c r="A990" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B990" s="2"/>
     </row>
     <row r="991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B991" s="2"/>
     </row>
     <row r="992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B992" s="2"/>
     </row>
     <row r="993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B993" s="2"/>
     </row>
     <row r="994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A994" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B994" s="2"/>
     </row>
     <row r="995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A995" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B995" s="2"/>
     </row>
     <row r="996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A996" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B996" s="2"/>
     </row>
     <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B997" s="2"/>
     </row>
     <row r="998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B998" s="2"/>
     </row>
     <row r="999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B999" s="2"/>
     </row>
     <row r="1000" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1000" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B1000" s="2"/>
     </row>
     <row r="1001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1001" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B1001" s="2"/>
     </row>
     <row r="1002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1002" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B1002" s="2"/>
     </row>
     <row r="1003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1003" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B1003" s="2"/>
     </row>
     <row r="1004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1004" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B1004" s="2"/>
     </row>
     <row r="1005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1005" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B1005" s="2"/>
     </row>
     <row r="1006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1006" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B1006" s="2"/>
     </row>
     <row r="1007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1007" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B1007" s="2"/>
     </row>
     <row r="1008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1008" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B1008" s="2"/>
     </row>
     <row r="1009" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1009" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B1009" s="2"/>
     </row>
     <row r="1010" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1010" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B1010" s="2"/>
     </row>
     <row r="1011" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1011" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B1011" s="2"/>
     </row>
     <row r="1012" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1012" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B1012" s="2"/>
     </row>
     <row r="1013" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1013" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B1013" s="2"/>
     </row>
     <row r="1014" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1014" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B1014" s="2"/>
     </row>
     <row r="1015" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1015" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B1015" s="2"/>
     </row>
     <row r="1016" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1016" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B1016" s="2"/>
     </row>
     <row r="1017" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1017" s="0" t="s">
@@ -10309,27 +10258,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:J40"/>
+  <dimension ref="A3:J88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D87" activeCellId="0" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="4"/>
       <c r="I3" s="0" t="s">
         <v>215</v>
       </c>
@@ -10338,22 +10290,22 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="6" t="n">
         <v>-18</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="6" t="n">
         <v>-18</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>-18</v>
       </c>
       <c r="I4" s="0" t="s">
@@ -10364,726 +10316,1170 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="6" t="n">
         <v>-17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>-17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>-17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="6" t="n">
         <v>-16</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>-16</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>-16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="6" t="n">
         <v>-15</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="6" t="n">
         <v>-15</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="6" t="n">
         <v>-15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="6" t="n">
         <v>-14</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>-14</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="6" t="n">
         <v>-14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="6" t="n">
         <v>-13</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>-13</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="6" t="n">
         <v>-13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="6" t="n">
         <v>-12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="6" t="n">
         <v>-12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="6" t="n">
         <v>-12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="6" t="n">
         <v>-11</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="6" t="n">
         <v>-11</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="6" t="n">
         <v>-11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="6" t="n">
         <v>-10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="6" t="n">
         <v>-10</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="6" t="n">
         <v>-10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="6" t="n">
         <v>-9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <v>-9</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="6" t="n">
         <v>-9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="6" t="n">
         <v>-8</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="6" t="n">
         <v>-8</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="6" t="n">
         <v>-8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="6" t="n">
         <v>-7</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="6" t="n">
         <v>-7</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="6" t="n">
         <v>-7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="6" t="n">
         <v>-6</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="6" t="n">
         <v>-6</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="6" t="n">
         <v>-6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="6" t="n">
         <v>-5</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <v>-5</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F17" s="7" t="n">
+      <c r="F17" s="6" t="n">
         <v>-5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="6" t="n">
         <v>-4</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="6" t="n">
         <v>-4</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="6" t="n">
         <v>-4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B19" s="6" t="n">
         <v>-3</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="7" t="n">
+      <c r="D19" s="6" t="n">
         <v>-3</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="F19" s="6" t="n">
         <v>-3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="6" t="n">
         <v>-2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="6" t="n">
         <v>-1</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="6" t="n">
         <v>-1</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="7" t="n">
+      <c r="F21" s="6" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10" t="s">
+      <c r="D22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D23" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="7" t="n">
+      <c r="F23" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="7" t="n">
+      <c r="B24" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D24" s="12" t="n">
+      <c r="D24" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="12" t="n">
+      <c r="F24" s="6" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="7" t="n">
+      <c r="B25" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="12" t="n">
+      <c r="D25" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="6" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="7" t="n">
+      <c r="B26" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D26" s="7" t="n">
+      <c r="D26" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F26" s="7" t="n">
+      <c r="F26" s="6" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B27" s="7" t="n">
+      <c r="B27" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F27" s="7" t="n">
+      <c r="F27" s="6" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="7" t="n">
+      <c r="B28" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="12" t="n">
+      <c r="D28" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="7" t="n">
+      <c r="F28" s="6" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B29" s="7" t="n">
+      <c r="B29" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D29" s="7" t="n">
+      <c r="D29" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="7" t="n">
+      <c r="F29" s="6" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B30" s="7" t="n">
+      <c r="B30" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D30" s="7" t="n">
+      <c r="D30" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F30" s="7" t="n">
+      <c r="F30" s="6" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B31" s="7" t="n">
+      <c r="B31" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D31" s="7" t="n">
+      <c r="D31" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="7" t="n">
+      <c r="F31" s="6" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="7" t="n">
+      <c r="B32" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="12" t="n">
+      <c r="D32" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="7" t="n">
+      <c r="F32" s="6" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B33" s="7" t="n">
+      <c r="B33" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D33" s="7" t="n">
+      <c r="D33" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F33" s="7" t="n">
+      <c r="F33" s="6" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B34" s="7" t="n">
+      <c r="B34" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D34" s="7" t="n">
+      <c r="D34" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F34" s="7" t="n">
+      <c r="F34" s="6" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B35" s="7" t="n">
+      <c r="B35" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D35" s="7" t="n">
+      <c r="D35" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F35" s="7" t="n">
+      <c r="F35" s="6" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="7" t="n">
+      <c r="B36" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="12" t="n">
+      <c r="D36" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="7" t="n">
+      <c r="F36" s="6" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B37" s="7" t="n">
+      <c r="B37" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D37" s="7" t="n">
+      <c r="D37" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F37" s="7" t="n">
+      <c r="F37" s="6" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B38" s="7" t="n">
+      <c r="B38" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D38" s="7" t="n">
+      <c r="D38" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F38" s="7" t="n">
+      <c r="F38" s="6" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B39" s="7" t="n">
+      <c r="B39" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="D39" s="7" t="n">
+      <c r="D39" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F39" s="7" t="n">
+      <c r="F39" s="6" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="14" t="n">
+      <c r="B40" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="16" t="n">
+      <c r="D40" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="14" t="n">
+      <c r="F40" s="11" t="n">
         <v>18</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A52,"""",",")</f>
+        <v>"de833e19",</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B53" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A53,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B54" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A54,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A55,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A56,"""",",")</f>
+        <v>"b09170bc",</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B57" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A57,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A58,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B59" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A59,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A60,"""",",")</f>
+        <v>"3f704a20",</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B61" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A61,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B62" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A62,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B63" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A63,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A64,"""",",")</f>
+        <v>"c85bef19",</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A65,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B66" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A66,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A67,"""",",")</f>
+        <v>"ad71085c",</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B68" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A68,"""",",")</f>
+        <v>"b88f46bf",</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A69,"""",",")</f>
+        <v>"bc1f93c3",</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A70,"""",",")</f>
+        <v>"ab2fdaa1",</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B71" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A71,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A72,"""",",")</f>
+        <v>"1cb3e57e",</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A73,"""",",")</f>
+        <v>"1195a71f",</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B74" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A74,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B75" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A75,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A76,"""",",")</f>
+        <v>"c3d5d3e2",</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B77" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A77,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B78" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A78,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B79" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A79,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B80" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A80,"""",",")</f>
+        <v>"3684fc19",</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B81" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A81,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B82" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A82,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B83" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A83,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A84,"""",",")</f>
+        <v>"aa0b5263",</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B85" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A85,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B86" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A86,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B87" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A87,"""",",")</f>
+        <v>"00000000",</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("""",A88,"""",",")</f>
+        <v>"9eed1400",</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>